<commit_message>
corrected numeracion.xlsx and config.R
</commit_message>
<xml_diff>
--- a/Numeracion.xlsx
+++ b/Numeracion.xlsx
@@ -1,17 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27417"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arturogf/cmdbclusteR/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="672" yWindow="96" windowWidth="20868" windowHeight="10056"/>
+    <workbookView xWindow="680" yWindow="460" windowWidth="20860" windowHeight="10060"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -127,16 +140,16 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -155,23 +168,23 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom/>
@@ -179,11 +192,11 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -228,28 +241,28 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -310,12 +323,12 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -345,12 +358,12 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -557,140 +570,140 @@
   <dimension ref="A2:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.21875" style="1" customWidth="1"/>
-    <col min="2" max="4" width="13.77734375" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="11.5546875" style="1"/>
+    <col min="1" max="1" width="9.1640625" style="1" customWidth="1"/>
+    <col min="2" max="4" width="13.83203125" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C2" s="11" t="s">
+    <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="C2" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="8" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B3" s="9" t="s">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B3" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="9">
+      <c r="C3" s="6">
+        <v>2</v>
+      </c>
+      <c r="D3" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B4" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="9">
+      <c r="C4" s="6">
+        <v>49</v>
+      </c>
+      <c r="D4" s="6">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B5" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="6">
+        <v>47</v>
+      </c>
+      <c r="D5" s="6">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B6" s="6" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B4" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="9">
-        <v>49</v>
-      </c>
-      <c r="D4" s="9">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B5" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" s="9">
-        <v>47</v>
-      </c>
-      <c r="D5" s="9">
+      <c r="C6" s="6">
+        <v>5</v>
+      </c>
+      <c r="D6" s="6">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B7" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="6">
+        <v>8</v>
+      </c>
+      <c r="D7" s="6">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B8" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="6">
+        <v>0</v>
+      </c>
+      <c r="D8" s="6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B9" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="6">
+        <v>3</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B10" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="6">
+        <v>4</v>
+      </c>
+      <c r="D10" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="9" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B6" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" s="9">
+      <c r="B11" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="9">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B7" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="9">
-        <v>8</v>
-      </c>
-      <c r="D7" s="9">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B8" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="9">
-        <v>0</v>
-      </c>
-      <c r="D8" s="9">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B9" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" s="9">
-        <v>3</v>
-      </c>
-      <c r="D9" s="9" t="s">
+      <c r="C11" s="7">
+        <v>50</v>
+      </c>
+      <c r="D11" s="6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B10" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" s="9">
-        <v>4</v>
-      </c>
-      <c r="D10" s="9">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" s="10">
-        <v>50</v>
-      </c>
-      <c r="D11" s="9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="4"/>
-      <c r="B12" s="7" t="s">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="10"/>
+      <c r="B12" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="8">
+      <c r="C12" s="5">
         <v>51</v>
       </c>
-      <c r="D12" s="8">
+      <c r="D12" s="5">
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="5"/>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="11"/>
       <c r="B13" s="3" t="s">
         <v>13</v>
       </c>
@@ -718,7 +731,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -730,7 +743,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
- move LOS calculation after the filling of blank dates. - fix bug in subsetPhewasVars()
</commit_message>
<xml_diff>
--- a/Numeracion.xlsx
+++ b/Numeracion.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="680" yWindow="460" windowWidth="20860" windowHeight="10060"/>
+    <workbookView xWindow="26840" yWindow="720" windowWidth="20860" windowHeight="10060"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -570,7 +570,7 @@
   <dimension ref="A2:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -645,35 +645,35 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B8" s="6" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C8" s="6">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D8" s="6">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B9" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="6">
+        <v>0</v>
+      </c>
+      <c r="D9" s="6">
         <v>6</v>
-      </c>
-      <c r="C9" s="6">
-        <v>3</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B10" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C10" s="6">
-        <v>4</v>
-      </c>
-      <c r="D10" s="6">
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>